<commit_message>
redo heatmaps with no outgr snp set
</commit_message>
<xml_diff>
--- a/05.analyses/demography/dadi/1D/cord/models/dadi_cord1D_results_summary.xlsx
+++ b/05.analyses/demography/dadi/1D/cord/models/dadi_cord1D_results_summary.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/kasey_pham_ufl_edu/Documents/Grad School Documents/Projects/eucalyptus-hybrid-resequencing/05.analyses/demography/dadi/1D/cord/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="258" documentId="8_{21408352-E5DB-40D9-AE77-F269512CD883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF89BDB0-56AF-433C-8D4C-389DF89AFCA0}"/>
+  <xr:revisionPtr revIDLastSave="344" documentId="8_{21408352-E5DB-40D9-AE77-F269512CD883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79D7F8AD-19CD-4E1E-8340-EEDB10E4FC06}"/>
   <bookViews>
-    <workbookView xWindow="-27510" yWindow="-9435" windowWidth="21195" windowHeight="12765" activeTab="3" xr2:uid="{2A3D79EE-876F-4CC7-84D9-EA1A1596E616}"/>
+    <workbookView xWindow="-23520" yWindow="-3870" windowWidth="19470" windowHeight="14175" activeTab="2" xr2:uid="{2A3D79EE-876F-4CC7-84D9-EA1A1596E616}"/>
   </bookViews>
   <sheets>
     <sheet name="all model results" sheetId="1" r:id="rId1"/>
     <sheet name="calc templ" sheetId="2" r:id="rId2"/>
-    <sheet name="03.two_epoch" sheetId="5" r:id="rId3"/>
-    <sheet name="05.three_epoch" sheetId="4" r:id="rId4"/>
+    <sheet name="Model 5" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,9 +28,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="43">
   <si>
     <t>02.growth</t>
   </si>
@@ -267,16 +263,19 @@
     </r>
   </si>
   <si>
-    <t>Run 5, Rep 66</t>
-  </si>
-  <si>
-    <t>Run 3, Rep 49</t>
-  </si>
-  <si>
-    <t>Run 3, Rep 8</t>
-  </si>
-  <si>
-    <t>Run 5, Rep 2</t>
+    <t>Run 1, Rep 5</t>
+  </si>
+  <si>
+    <t>Run 2, Rep 61</t>
+  </si>
+  <si>
+    <t>Run 2, Rep 45</t>
+  </si>
+  <si>
+    <t>Run 2, Rep 73</t>
+  </si>
+  <si>
+    <t>05 - Three Epoch</t>
   </si>
 </sst>
 </file>
@@ -717,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -728,8 +727,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -777,8 +774,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1164,44 +1162,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1123D7EB-ECD6-4C25-BAEF-EFE90AE1E5C4}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.90625" customWidth="1"/>
+    <col min="7" max="7" width="10.36328125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" customWidth="1"/>
+    <col min="9" max="9" width="10.08984375" customWidth="1"/>
+    <col min="10" max="10" width="8.90625" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
-    <col min="12" max="12" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="49" t="s">
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="51"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="50"/>
       <c r="L1" s="9" t="s">
         <v>7</v>
       </c>
@@ -1221,93 +1219,93 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="45">
-        <v>-4358.74</v>
+      <c r="B2" s="46">
+        <v>-7399.12</v>
       </c>
       <c r="C2">
-        <v>-4358.82</v>
+        <v>-7399.26</v>
       </c>
       <c r="D2">
-        <v>-4358.8500000000004</v>
+        <v>-7399.19</v>
       </c>
       <c r="E2">
-        <v>-4358.75</v>
-      </c>
-      <c r="F2" s="47">
-        <v>-4358.7</v>
-      </c>
-      <c r="G2">
-        <v>8721.48</v>
+        <v>-7399.12</v>
+      </c>
+      <c r="F2" s="2">
+        <v>-7399.13</v>
+      </c>
+      <c r="G2" s="45">
+        <v>14802.24</v>
       </c>
       <c r="H2">
-        <v>8721.64</v>
+        <v>14802.52</v>
       </c>
       <c r="I2">
-        <v>8721.7000000000007</v>
+        <v>14802.38</v>
       </c>
       <c r="J2">
-        <v>8721.5</v>
-      </c>
-      <c r="K2" s="10">
-        <v>8721.4</v>
+        <v>14802.24</v>
+      </c>
+      <c r="K2">
+        <v>14802.26</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>38</v>
       </c>
       <c r="M2">
-        <v>590241.9</v>
+        <v>930770.7</v>
       </c>
       <c r="N2">
         <v>0.01</v>
       </c>
       <c r="P2">
-        <v>4.6300000000000001E-2</v>
+        <v>4.6100000000000002E-2</v>
       </c>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="45">
-        <v>-4169.83</v>
-      </c>
-      <c r="C3">
-        <v>-4169.87</v>
-      </c>
-      <c r="D3" s="10">
-        <v>-4169.79</v>
+      <c r="B3" s="43">
+        <v>-7092.79</v>
+      </c>
+      <c r="C3" s="45">
+        <v>-7092.77</v>
+      </c>
+      <c r="D3">
+        <v>-7093.18</v>
       </c>
       <c r="E3">
-        <v>-4170.18</v>
+        <v>-7092.97</v>
       </c>
       <c r="F3" s="2">
-        <v>-4169.99</v>
+        <v>-7092.9</v>
       </c>
       <c r="G3">
-        <v>8343.66</v>
-      </c>
-      <c r="H3">
-        <v>8343.74</v>
-      </c>
-      <c r="I3" s="10">
-        <v>8343.58</v>
+        <v>14189.58</v>
+      </c>
+      <c r="H3" s="45">
+        <v>14189.54</v>
+      </c>
+      <c r="I3">
+        <v>14190.36</v>
       </c>
       <c r="J3">
-        <v>8344.36</v>
+        <v>14189.94</v>
       </c>
       <c r="K3">
-        <v>8343.98</v>
+        <v>14189.8</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>39</v>
       </c>
       <c r="M3">
-        <v>613341.1</v>
+        <v>969599.1</v>
       </c>
       <c r="N3">
         <v>0.01</v>
@@ -1317,108 +1315,108 @@
       </c>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="45">
-        <v>-4356.08</v>
-      </c>
-      <c r="C4">
-        <v>-4252.99</v>
-      </c>
-      <c r="D4" s="10">
-        <v>-4243.0600000000004</v>
+      <c r="B4" s="43">
+        <v>-7388.91</v>
+      </c>
+      <c r="C4" s="45">
+        <v>-7358.44</v>
+      </c>
+      <c r="D4">
+        <v>-7399.08</v>
       </c>
       <c r="E4">
-        <v>-4359</v>
+        <v>-7388.11</v>
       </c>
       <c r="F4" s="2">
-        <v>-4359.2299999999996</v>
+        <v>-7399.41</v>
       </c>
       <c r="G4">
-        <v>8718.16</v>
-      </c>
-      <c r="H4">
-        <v>8511.98</v>
-      </c>
-      <c r="I4" s="10">
-        <v>8492.1200000000008</v>
+        <v>14783.82</v>
+      </c>
+      <c r="H4" s="45">
+        <v>14722.88</v>
+      </c>
+      <c r="I4">
+        <v>14804.16</v>
       </c>
       <c r="J4">
-        <v>8724</v>
+        <v>14782.22</v>
       </c>
       <c r="K4">
-        <v>8724.4599999999991</v>
+        <v>14804.82</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>40</v>
       </c>
       <c r="M4">
-        <v>617885.69999999995</v>
+        <v>924199.6</v>
       </c>
       <c r="N4">
-        <v>1.8200000000000001E-2</v>
+        <v>0.1012</v>
       </c>
       <c r="O4">
         <v>0.01</v>
       </c>
       <c r="P4">
-        <v>1.35E-2</v>
+        <v>2.4799999999999999E-2</v>
       </c>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="46">
-        <v>-3900.93</v>
-      </c>
-      <c r="C5" s="3">
-        <v>-3385.34</v>
+      <c r="B5" s="44">
+        <v>-6552</v>
+      </c>
+      <c r="C5" s="47">
+        <v>-5272.02</v>
       </c>
       <c r="D5" s="3">
-        <v>-3635.33</v>
+        <v>-5411.22</v>
       </c>
       <c r="E5" s="3">
-        <v>-3097.8</v>
-      </c>
-      <c r="F5" s="48">
-        <v>-3084.96</v>
+        <v>-5324.44</v>
+      </c>
+      <c r="F5" s="4">
+        <v>-5316.6</v>
       </c>
       <c r="G5" s="3">
-        <v>7809.86</v>
-      </c>
-      <c r="H5" s="3">
-        <v>6778.68</v>
+        <v>13112</v>
+      </c>
+      <c r="H5" s="47">
+        <v>10552.04</v>
       </c>
       <c r="I5" s="3">
-        <v>7278.66</v>
+        <v>10830.44</v>
       </c>
       <c r="J5" s="3">
-        <v>6203.6</v>
-      </c>
-      <c r="K5" s="11">
-        <v>6177.92</v>
+        <v>10656.88</v>
+      </c>
+      <c r="K5" s="3">
+        <v>10641.2</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>41</v>
       </c>
       <c r="M5" s="3">
-        <v>63254.2</v>
+        <v>91424.01</v>
       </c>
       <c r="N5" s="3">
-        <v>27.653500000000001</v>
+        <v>26.566500000000001</v>
       </c>
       <c r="O5" s="3">
-        <v>1.4E-2</v>
+        <v>1.01E-2</v>
       </c>
       <c r="P5" s="3">
-        <v>24.8504</v>
+        <v>23.965299999999999</v>
       </c>
       <c r="Q5" s="4">
-        <v>2.1299999999999999E-2</v>
+        <v>1.41E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1427,7 +1425,6 @@
     <mergeCell ref="G1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1436,88 +1433,88 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="8.21875" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" customWidth="1"/>
-    <col min="5" max="5" width="4.109375" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" customWidth="1"/>
-    <col min="7" max="7" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="4.77734375" customWidth="1"/>
-    <col min="10" max="10" width="6.88671875" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" customWidth="1"/>
-    <col min="12" max="12" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1"/>
+    <col min="5" max="5" width="4.08984375" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" customWidth="1"/>
+    <col min="7" max="7" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" customWidth="1"/>
+    <col min="9" max="9" width="4.7265625" customWidth="1"/>
+    <col min="10" max="10" width="6.90625" customWidth="1"/>
+    <col min="11" max="11" width="13.08984375" customWidth="1"/>
+    <col min="12" max="12" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="56"/>
-      <c r="F3" s="57" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="55"/>
+      <c r="F3" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="54"/>
-      <c r="H3" s="58"/>
-      <c r="J3" s="57" t="s">
+      <c r="G3" s="53"/>
+      <c r="H3" s="57"/>
+      <c r="J3" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="58"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13" t="s">
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="57"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="13" t="s">
+      <c r="J4" s="16"/>
+      <c r="K4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="67.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:13" ht="67.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1526,157 +1523,157 @@
       <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="F5" s="21" t="s">
+      <c r="D5" s="18"/>
+      <c r="F5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="18">
         <v>4.9300000000000001E-9</v>
       </c>
-      <c r="J5" s="44" t="s">
+      <c r="J5" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="24"/>
-      <c r="M5" s="25">
+      <c r="L5" s="22"/>
+      <c r="M5" s="23">
         <f>D5/(4*H5*H6*H9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="60" t="s">
+    <row r="6" spans="1:13" ht="29.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="59" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="26"/>
-      <c r="F6" s="21" t="s">
+      <c r="D6" s="24"/>
+      <c r="F6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="20">
-        <v>10</v>
-      </c>
-      <c r="J6" s="60" t="s">
+      <c r="H6" s="18">
+        <v>50</v>
+      </c>
+      <c r="J6" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="42" t="s">
+      <c r="K6" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="L6" s="27"/>
-      <c r="M6" s="28">
+      <c r="L6" s="25"/>
+      <c r="M6" s="26">
         <f>D6*M5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="62"/>
+    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="61"/>
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="20"/>
-      <c r="F7" s="29" t="s">
+      <c r="D7" s="18"/>
+      <c r="F7" s="27" t="s">
         <v>28</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="24">
         <v>603301446</v>
       </c>
-      <c r="J7" s="62"/>
-      <c r="K7" s="33" t="s">
+      <c r="J7" s="61"/>
+      <c r="K7" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="L7" s="34"/>
-      <c r="M7" s="35">
+      <c r="L7" s="32"/>
+      <c r="M7" s="33">
         <f>D7*M5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="60" t="s">
+    <row r="8" spans="1:13" ht="27.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="59" t="s">
         <v>32</v>
       </c>
       <c r="B8" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="26"/>
-      <c r="F8" s="29" t="s">
+      <c r="D8" s="24"/>
+      <c r="F8" s="27" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="2"/>
-      <c r="H8" s="26">
-        <f>(8732510/600502230)*(1066040/1226278)</f>
-        <v>1.2641803364126243E-2</v>
-      </c>
-      <c r="J8" s="60" t="s">
+      <c r="H8" s="24">
+        <f>(15859769/599899923)*(1736464/(1839839+106915))</f>
+        <v>2.3581572371007518E-2</v>
+      </c>
+      <c r="J8" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="42" t="s">
+      <c r="K8" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="27" t="s">
+      <c r="L8" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="M8" s="28">
+      <c r="M8" s="26">
         <f>2*D8*M5*H6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="61"/>
-      <c r="B9" s="36" t="s">
+    <row r="9" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="60"/>
+      <c r="B9" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
-      <c r="F9" s="30" t="s">
+      <c r="C9" s="35"/>
+      <c r="D9" s="36"/>
+      <c r="F9" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="30">
         <f>H7*H8</f>
-        <v>7626818.2496250272</v>
-      </c>
-      <c r="J9" s="61"/>
-      <c r="K9" s="39" t="s">
+        <v>14226796.710382484</v>
+      </c>
+      <c r="J9" s="60"/>
+      <c r="K9" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="31" t="s">
+      <c r="L9" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="M9" s="40">
+      <c r="M9" s="38">
         <f>2*D9*M5*H6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J10" s="59"/>
-      <c r="M10" s="43"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J11" s="59"/>
-      <c r="M11" s="43"/>
-    </row>
-    <row r="12" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="M14" s="43"/>
+    <row r="10" spans="1:13" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J10" s="58"/>
+      <c r="M10" s="41"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="J11" s="58"/>
+      <c r="M11" s="41"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="M14" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1695,365 +1692,94 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CECD055-A0A2-42FF-9512-FD95299429B8}">
-  <dimension ref="A1:M14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="8.21875" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" customWidth="1"/>
-    <col min="5" max="5" width="4.109375" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" customWidth="1"/>
-    <col min="7" max="7" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="4.77734375" customWidth="1"/>
-    <col min="10" max="10" width="6.88671875" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" customWidth="1"/>
-    <col min="12" max="12" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="63" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="56"/>
-      <c r="F3" s="57" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="54"/>
-      <c r="H3" s="58"/>
-      <c r="J3" s="57" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="58"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="67.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="20">
-        <v>613341.1</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="20">
-        <v>4.9300000000000001E-9</v>
-      </c>
-      <c r="J5" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="24"/>
-      <c r="M5" s="25">
-        <f>D5/(4*H5*H6*H9)</f>
-        <v>407804.26175150205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="20">
-        <v>10</v>
-      </c>
-      <c r="J6" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="27"/>
-      <c r="M6" s="28">
-        <f>D6*M5</f>
-        <v>4078.0426175150205</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="62"/>
-      <c r="B7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="20"/>
-      <c r="F7" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="26">
-        <v>603301446</v>
-      </c>
-      <c r="J7" s="62"/>
-      <c r="K7" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="34"/>
-      <c r="M7" s="35">
-        <f>D7*M5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="60" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="26">
-        <f>(8732510/600502230)*(1066040/1226278)</f>
-        <v>1.2641803364126243E-2</v>
-      </c>
-      <c r="J8" s="60" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="L8" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="M8" s="28">
-        <f>2*D8*M5*H6</f>
-        <v>81560.852350300411</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="61"/>
-      <c r="B9" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
-      <c r="F9" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="32">
-        <f>H7*H8</f>
-        <v>7626818.2496250272</v>
-      </c>
-      <c r="J9" s="61"/>
-      <c r="K9" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="L9" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" s="40">
-        <f>2*D9*M5*H6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J10" s="59"/>
-      <c r="M10" s="43"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J11" s="59"/>
-      <c r="M11" s="43"/>
-    </row>
-    <row r="12" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="M14" s="43"/>
-    </row>
-  </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="J6:J7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477B02B9-F3EB-4652-BD38-9CEDC80D3E86}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF2F61F2-3A38-4AED-8FEA-6EC755D0677C}">
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="8.21875" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" customWidth="1"/>
-    <col min="5" max="5" width="4.109375" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" customWidth="1"/>
-    <col min="7" max="7" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="4.77734375" customWidth="1"/>
-    <col min="10" max="10" width="6.88671875" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" customWidth="1"/>
-    <col min="12" max="12" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1"/>
+    <col min="5" max="5" width="4.08984375" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" customWidth="1"/>
+    <col min="7" max="7" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" customWidth="1"/>
+    <col min="9" max="9" width="4.7265625" customWidth="1"/>
+    <col min="10" max="10" width="6.90625" customWidth="1"/>
+    <col min="11" max="11" width="13.08984375" customWidth="1"/>
+    <col min="12" max="12" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="63" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="B1" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="56"/>
-      <c r="F3" s="57" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="55"/>
+      <c r="F3" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="54"/>
-      <c r="H3" s="58"/>
-      <c r="J3" s="57" t="s">
+      <c r="G3" s="53"/>
+      <c r="H3" s="57"/>
+      <c r="J3" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="58"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13" t="s">
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="57"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="13" t="s">
+      <c r="J4" s="16"/>
+      <c r="K4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="67.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:13" ht="67.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -2062,167 +1788,168 @@
       <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="20">
-        <v>63254.2</v>
-      </c>
-      <c r="F5" s="21" t="s">
+      <c r="D5" s="18">
+        <v>91424.01</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="20">
-        <v>4.9300000000000001E-9</v>
-      </c>
-      <c r="J5" s="44" t="s">
+      <c r="H5" s="18">
+        <f>0.0000000493/100</f>
+        <v>4.9299999999999995E-10</v>
+      </c>
+      <c r="J5" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="24"/>
-      <c r="M5" s="25">
+      <c r="L5" s="22"/>
+      <c r="M5" s="23">
         <f>D5/(4*H5*H6*H9)</f>
-        <v>42057.07449522274</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="60" t="s">
+        <v>65174.277501125252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="29.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="59" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="26">
-        <v>27.653500000000001</v>
-      </c>
-      <c r="F6" s="21" t="s">
+      <c r="D6" s="24">
+        <v>26.566500000000001</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="20">
-        <v>10</v>
-      </c>
-      <c r="J6" s="60" t="s">
+      <c r="H6" s="18">
+        <v>50</v>
+      </c>
+      <c r="J6" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="42" t="s">
+      <c r="K6" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="L6" s="27"/>
-      <c r="M6" s="28">
+      <c r="L6" s="25"/>
+      <c r="M6" s="26">
         <f>D6*M5</f>
-        <v>1163025.3095536421</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="62"/>
+        <v>1731452.4432336441</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="61"/>
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="20">
-        <v>1.4E-2</v>
-      </c>
-      <c r="F7" s="29" t="s">
+      <c r="D7" s="18">
+        <v>1.01E-2</v>
+      </c>
+      <c r="F7" s="27" t="s">
         <v>28</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="24">
         <v>603301446</v>
       </c>
-      <c r="J7" s="62"/>
-      <c r="K7" s="33" t="s">
+      <c r="J7" s="61"/>
+      <c r="K7" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="L7" s="34"/>
-      <c r="M7" s="35">
+      <c r="L7" s="32"/>
+      <c r="M7" s="33">
         <f>D7*M5</f>
-        <v>588.79904293311836</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="60" t="s">
+        <v>658.26020276136501</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="27.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="59" t="s">
         <v>32</v>
       </c>
       <c r="B8" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="26">
-        <v>24.8504</v>
-      </c>
-      <c r="F8" s="29" t="s">
+      <c r="D8" s="24">
+        <v>23.965299999999999</v>
+      </c>
+      <c r="F8" s="27" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="2"/>
-      <c r="H8" s="26">
-        <f>(8732510/600502230)*(1066040/1226278)</f>
-        <v>1.2641803364126243E-2</v>
-      </c>
-      <c r="J8" s="60" t="s">
+      <c r="H8" s="24">
+        <f>(15859769/599899923)*(1736464/(1839839+106915))</f>
+        <v>2.3581572371007518E-2</v>
+      </c>
+      <c r="J8" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="42" t="s">
+      <c r="K8" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="27" t="s">
+      <c r="L8" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="M8" s="28">
+      <c r="M8" s="26">
         <f>2*D8*M5*H6</f>
-        <v>20902702.480721664</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="61"/>
-      <c r="B9" s="36" t="s">
+        <v>156192111.2597717</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="60"/>
+      <c r="B9" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="38">
-        <v>2.1299999999999999E-2</v>
-      </c>
-      <c r="F9" s="30" t="s">
+      <c r="C9" s="35"/>
+      <c r="D9" s="36">
+        <v>1.41E-2</v>
+      </c>
+      <c r="F9" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="30">
         <f>H7*H8</f>
-        <v>7626818.2496250272</v>
-      </c>
-      <c r="J9" s="61"/>
-      <c r="K9" s="39" t="s">
+        <v>14226796.710382484</v>
+      </c>
+      <c r="J9" s="60"/>
+      <c r="K9" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="31" t="s">
+      <c r="L9" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="M9" s="40">
+      <c r="M9" s="38">
         <f>2*D9*M5*H6</f>
-        <v>17916.31373496489</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J10" s="59"/>
-      <c r="M10" s="43"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J11" s="59"/>
-      <c r="M11" s="43"/>
-    </row>
-    <row r="12" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="M14" s="43"/>
+        <v>91895.731276586608</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J10" s="58"/>
+      <c r="M10" s="41"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="J11" s="58"/>
+      <c r="M11" s="41"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="M14" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
finished 1D summations and redid 2D calculations with corrected gentimes
</commit_message>
<xml_diff>
--- a/05.analyses/demography/dadi/1D/cord/models/dadi_cord1D_results_summary.xlsx
+++ b/05.analyses/demography/dadi/1D/cord/models/dadi_cord1D_results_summary.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/kasey_pham_ufl_edu/Documents/Grad School Documents/Projects/eucalyptus-hybrid-resequencing/05.analyses/demography/dadi/1D/cord/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="344" documentId="8_{21408352-E5DB-40D9-AE77-F269512CD883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79D7F8AD-19CD-4E1E-8340-EEDB10E4FC06}"/>
+  <xr:revisionPtr revIDLastSave="380" documentId="8_{21408352-E5DB-40D9-AE77-F269512CD883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2471D2B4-1975-4840-8376-08477C84E082}"/>
   <bookViews>
-    <workbookView xWindow="-23520" yWindow="-3870" windowWidth="19470" windowHeight="14175" activeTab="2" xr2:uid="{2A3D79EE-876F-4CC7-84D9-EA1A1596E616}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{2A3D79EE-876F-4CC7-84D9-EA1A1596E616}"/>
   </bookViews>
   <sheets>
     <sheet name="all model results" sheetId="1" r:id="rId1"/>
     <sheet name="calc templ" sheetId="2" r:id="rId2"/>
     <sheet name="Model 5" sheetId="3" r:id="rId3"/>
+    <sheet name="Model 3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="50">
   <si>
     <t>02.growth</t>
   </si>
@@ -276,6 +277,53 @@
   </si>
   <si>
     <t>05 - Three Epoch</t>
+  </si>
+  <si>
+    <t>UNCERTAINTY ESTIMATES</t>
+  </si>
+  <si>
+    <t>95% CONFIDENCE INTERVALS</t>
+  </si>
+  <si>
+    <t>Lower Bound</t>
+  </si>
+  <si>
+    <t>Upper Bound</t>
+  </si>
+  <si>
+    <r>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Two Epoch</t>
   </si>
 </sst>
 </file>
@@ -323,7 +371,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -348,8 +396,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="32">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -712,11 +784,127 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -774,9 +962,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -822,6 +1007,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1163,7 +1389,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1186,20 +1412,20 @@
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="48" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="50"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="47"/>
       <c r="L1" s="9" t="s">
         <v>7</v>
       </c>
@@ -1223,7 +1449,7 @@
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="46">
+      <c r="B2" s="87">
         <v>-7399.12</v>
       </c>
       <c r="C2">
@@ -1238,7 +1464,7 @@
       <c r="F2" s="2">
         <v>-7399.13</v>
       </c>
-      <c r="G2" s="45">
+      <c r="G2" s="88">
         <v>14802.24</v>
       </c>
       <c r="H2">
@@ -1274,7 +1500,7 @@
       <c r="B3" s="43">
         <v>-7092.79</v>
       </c>
-      <c r="C3" s="45">
+      <c r="C3" s="85">
         <v>-7092.77</v>
       </c>
       <c r="D3">
@@ -1289,7 +1515,7 @@
       <c r="G3">
         <v>14189.58</v>
       </c>
-      <c r="H3" s="45">
+      <c r="H3" s="85">
         <v>14189.54</v>
       </c>
       <c r="I3">
@@ -1322,7 +1548,7 @@
       <c r="B4" s="43">
         <v>-7388.91</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="86">
         <v>-7358.44</v>
       </c>
       <c r="D4">
@@ -1337,7 +1563,7 @@
       <c r="G4">
         <v>14783.82</v>
       </c>
-      <c r="H4" s="45">
+      <c r="H4" s="86">
         <v>14722.88</v>
       </c>
       <c r="I4">
@@ -1373,7 +1599,7 @@
       <c r="B5" s="44">
         <v>-6552</v>
       </c>
-      <c r="C5" s="47">
+      <c r="C5" s="84">
         <v>-5272.02</v>
       </c>
       <c r="D5" s="3">
@@ -1388,7 +1614,7 @@
       <c r="G5" s="3">
         <v>13112</v>
       </c>
-      <c r="H5" s="47">
+      <c r="H5" s="84">
         <v>10552.04</v>
       </c>
       <c r="I5" s="3">
@@ -1430,10 +1656,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AACE7548-1ED1-43B1-8D49-BE726A669DE7}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1451,38 +1677,56 @@
     <col min="11" max="11" width="13.08984375" customWidth="1"/>
     <col min="12" max="12" width="7.08984375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.90625" customWidth="1"/>
+    <col min="14" max="14" width="4.453125" customWidth="1"/>
+    <col min="16" max="16" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.54296875" customWidth="1"/>
+    <col min="18" max="18" width="4" customWidth="1"/>
+    <col min="22" max="22" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="52" t="s">
+    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="55"/>
-      <c r="F3" s="56" t="s">
+      <c r="B3" s="50"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="52"/>
+      <c r="F3" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="57"/>
-      <c r="J3" s="56" t="s">
+      <c r="G3" s="50"/>
+      <c r="H3" s="54"/>
+      <c r="J3" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="57"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="54"/>
+      <c r="O3" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="S3" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="50"/>
+      <c r="U3" s="50"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="54"/>
+    </row>
+    <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
         <v>17</v>
@@ -1512,8 +1756,28 @@
       <c r="M4" s="15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="67.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="O4" s="61"/>
+      <c r="P4" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" s="27"/>
+      <c r="T4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U4" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" s="65" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="67.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="17" t="s">
         <v>20</v>
       </c>
@@ -1544,9 +1808,31 @@
         <f>D5/(4*H5*H6*H9)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="29.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="59" t="s">
+      <c r="O5" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="18"/>
+      <c r="S5" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="T5" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="U5" s="69"/>
+      <c r="V5" s="70">
+        <f>(D5 - 2*Q5)/(4*H5*H6*H9)</f>
+        <v>0</v>
+      </c>
+      <c r="W5" s="71">
+        <f>(D5+2*Q5)/(4*H5*H6*H9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="29.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="56" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">
@@ -1561,9 +1847,9 @@
         <v>27</v>
       </c>
       <c r="H6" s="18">
-        <v>50</v>
-      </c>
-      <c r="J6" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="J6" s="56" t="s">
         <v>24</v>
       </c>
       <c r="K6" s="40" t="s">
@@ -1574,9 +1860,31 @@
         <f>D6*M5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="61"/>
+      <c r="O6" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" s="24"/>
+      <c r="S6" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="T6" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="U6" s="74"/>
+      <c r="V6" s="75">
+        <f>(D6-2*Q6)*M5</f>
+        <v>0</v>
+      </c>
+      <c r="W6" s="76">
+        <f>(D6+2*Q6)*M5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="58"/>
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
@@ -1591,7 +1899,7 @@
       <c r="H7" s="24">
         <v>603301446</v>
       </c>
-      <c r="J7" s="61"/>
+      <c r="J7" s="58"/>
       <c r="K7" s="31" t="s">
         <v>35</v>
       </c>
@@ -1600,9 +1908,27 @@
         <f>D7*M5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="27.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="59" t="s">
+      <c r="O7" s="58"/>
+      <c r="P7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="18"/>
+      <c r="S7" s="77"/>
+      <c r="T7" s="78" t="s">
+        <v>35</v>
+      </c>
+      <c r="U7" s="32"/>
+      <c r="V7" s="79">
+        <f>(D7-2*Q7)*M5</f>
+        <v>0</v>
+      </c>
+      <c r="W7" s="33">
+        <f>(D7+2*Q7)*M5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="27.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="56" t="s">
         <v>32</v>
       </c>
       <c r="B8" t="s">
@@ -1618,7 +1944,7 @@
         <f>(15859769/599899923)*(1736464/(1839839+106915))</f>
         <v>2.3581572371007518E-2</v>
       </c>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="56" t="s">
         <v>32</v>
       </c>
       <c r="K8" s="40" t="s">
@@ -1631,9 +1957,33 @@
         <f>2*D8*M5*H6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="60"/>
+      <c r="O8" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="80" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q8" s="24"/>
+      <c r="S8" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="T8" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="U8" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="V8" s="81">
+        <f>2*(D8-2*Q8)*M5*H6</f>
+        <v>0</v>
+      </c>
+      <c r="W8" s="26">
+        <f>2*(D8+2*Q8)*M5*H6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="57"/>
       <c r="B9" s="34" t="s">
         <v>37</v>
       </c>
@@ -1649,7 +1999,7 @@
         <f>H7*H8</f>
         <v>14226796.710382484</v>
       </c>
-      <c r="J9" s="60"/>
+      <c r="J9" s="57"/>
       <c r="K9" s="37" t="s">
         <v>37</v>
       </c>
@@ -1660,23 +2010,49 @@
         <f>2*D9*M5*H6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="J10" s="58"/>
+      <c r="O9" s="57"/>
+      <c r="P9" s="82" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q9" s="36"/>
+      <c r="S9" s="57"/>
+      <c r="T9" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="U9" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="V9" s="83">
+        <f>2*(D9-2*Q9)*M5*H6</f>
+        <v>0</v>
+      </c>
+      <c r="W9" s="38">
+        <f>2*(D9+2*Q9)*M5*H6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J10" s="55"/>
       <c r="M10" s="41"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="J11" s="58"/>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="J11" s="55"/>
       <c r="M11" s="41"/>
     </row>
-    <row r="12" spans="1:13" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="39"/>
       <c r="J14" s="39"/>
       <c r="M14" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="15">
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="S3:W3"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="S8:S9"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="F3:H3"/>
@@ -1693,10 +2069,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF2F61F2-3A38-4AED-8FEA-6EC755D0677C}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1714,40 +2090,57 @@
     <col min="11" max="11" width="13.08984375" customWidth="1"/>
     <col min="12" max="12" width="7.08984375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.90625" customWidth="1"/>
+    <col min="14" max="14" width="4.7265625" customWidth="1"/>
+    <col min="16" max="16" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.6328125" customWidth="1"/>
+    <col min="18" max="18" width="4.6328125" customWidth="1"/>
+    <col min="22" max="23" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="52" t="s">
+    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="55"/>
-      <c r="F3" s="56" t="s">
+      <c r="B3" s="50"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="52"/>
+      <c r="F3" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="57"/>
-      <c r="J3" s="56" t="s">
+      <c r="G3" s="50"/>
+      <c r="H3" s="54"/>
+      <c r="J3" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="57"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="54"/>
+      <c r="O3" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="S3" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="50"/>
+      <c r="U3" s="50"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="54"/>
+    </row>
+    <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
         <v>17</v>
@@ -1777,8 +2170,28 @@
       <c r="M4" s="15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="67.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="O4" s="61"/>
+      <c r="P4" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" s="27"/>
+      <c r="T4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U4" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" s="65" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="67.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="17" t="s">
         <v>20</v>
       </c>
@@ -1810,11 +2223,33 @@
       <c r="L5" s="22"/>
       <c r="M5" s="23">
         <f>D5/(4*H5*H6*H9)</f>
-        <v>65174.277501125252</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="29.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="59" t="s">
+        <v>32587.138750562626</v>
+      </c>
+      <c r="O5" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="18"/>
+      <c r="S5" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="T5" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="U5" s="69"/>
+      <c r="V5" s="70">
+        <f>(D5 - 2*Q5)/(4*H5*H6*H9)</f>
+        <v>32587.138750562626</v>
+      </c>
+      <c r="W5" s="71">
+        <f>(D5+2*Q5)/(4*H5*H6*H9)</f>
+        <v>32587.138750562626</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="29.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="56" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">
@@ -1831,9 +2266,9 @@
         <v>27</v>
       </c>
       <c r="H6" s="18">
-        <v>50</v>
-      </c>
-      <c r="J6" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="J6" s="56" t="s">
         <v>24</v>
       </c>
       <c r="K6" s="40" t="s">
@@ -1842,11 +2277,33 @@
       <c r="L6" s="25"/>
       <c r="M6" s="26">
         <f>D6*M5</f>
-        <v>1731452.4432336441</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="61"/>
+        <v>865726.22161682206</v>
+      </c>
+      <c r="O6" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" s="24"/>
+      <c r="S6" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="T6" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="U6" s="74"/>
+      <c r="V6" s="75">
+        <f>(D6-2*Q6)*M5</f>
+        <v>865726.22161682206</v>
+      </c>
+      <c r="W6" s="76">
+        <f>(D6+2*Q6)*M5</f>
+        <v>865726.22161682206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="58"/>
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
@@ -1863,18 +2320,36 @@
       <c r="H7" s="24">
         <v>603301446</v>
       </c>
-      <c r="J7" s="61"/>
+      <c r="J7" s="58"/>
       <c r="K7" s="31" t="s">
         <v>35</v>
       </c>
       <c r="L7" s="32"/>
       <c r="M7" s="33">
         <f>D7*M5</f>
-        <v>658.26020276136501</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="27.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="59" t="s">
+        <v>329.1301013806825</v>
+      </c>
+      <c r="O7" s="58"/>
+      <c r="P7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="18"/>
+      <c r="S7" s="77"/>
+      <c r="T7" s="78" t="s">
+        <v>35</v>
+      </c>
+      <c r="U7" s="32"/>
+      <c r="V7" s="79">
+        <f>(D7-2*Q7)*M5</f>
+        <v>329.1301013806825</v>
+      </c>
+      <c r="W7" s="33">
+        <f>(D7+2*Q7)*M5</f>
+        <v>329.1301013806825</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="27.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="56" t="s">
         <v>32</v>
       </c>
       <c r="B8" t="s">
@@ -1892,7 +2367,7 @@
         <f>(15859769/599899923)*(1736464/(1839839+106915))</f>
         <v>2.3581572371007518E-2</v>
       </c>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="56" t="s">
         <v>32</v>
       </c>
       <c r="K8" s="40" t="s">
@@ -1905,9 +2380,33 @@
         <f>2*D8*M5*H6</f>
         <v>156192111.2597717</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="60"/>
+      <c r="O8" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="80" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q8" s="24"/>
+      <c r="S8" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="T8" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="U8" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="V8" s="81">
+        <f>2*(D8-2*Q8)*M5*H6</f>
+        <v>156192111.2597717</v>
+      </c>
+      <c r="W8" s="26">
+        <f>2*(D8+2*Q8)*M5*H6</f>
+        <v>156192111.2597717</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="57"/>
       <c r="B9" s="34" t="s">
         <v>37</v>
       </c>
@@ -1925,7 +2424,7 @@
         <f>H7*H8</f>
         <v>14226796.710382484</v>
       </c>
-      <c r="J9" s="60"/>
+      <c r="J9" s="57"/>
       <c r="K9" s="37" t="s">
         <v>37</v>
       </c>
@@ -1936,23 +2435,49 @@
         <f>2*D9*M5*H6</f>
         <v>91895.731276586608</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="J10" s="58"/>
+      <c r="O9" s="57"/>
+      <c r="P9" s="82" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q9" s="36"/>
+      <c r="S9" s="57"/>
+      <c r="T9" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="U9" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="V9" s="83">
+        <f>2*(D9-2*Q9)*M5*H6</f>
+        <v>91895.731276586608</v>
+      </c>
+      <c r="W9" s="38">
+        <f>2*(D9+2*Q9)*M5*H6</f>
+        <v>91895.731276586608</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J10" s="55"/>
       <c r="M10" s="41"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="J11" s="58"/>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="J11" s="55"/>
       <c r="M11" s="41"/>
     </row>
-    <row r="12" spans="1:13" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="39"/>
       <c r="J14" s="39"/>
       <c r="M14" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="15">
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="S3:W3"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="S8:S9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="J10:J11"/>
@@ -1965,4 +2490,431 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED4A405-5A85-4992-8768-5EA27FBA628E}">
+  <dimension ref="A1:W14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1"/>
+    <col min="5" max="5" width="4.08984375" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" customWidth="1"/>
+    <col min="7" max="7" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" customWidth="1"/>
+    <col min="9" max="9" width="4.7265625" customWidth="1"/>
+    <col min="10" max="10" width="6.90625" customWidth="1"/>
+    <col min="11" max="11" width="13.08984375" customWidth="1"/>
+    <col min="12" max="12" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.90625" customWidth="1"/>
+    <col min="14" max="14" width="4.453125" customWidth="1"/>
+    <col min="16" max="16" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.54296875" customWidth="1"/>
+    <col min="18" max="18" width="4" customWidth="1"/>
+    <col min="22" max="22" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="50"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="52"/>
+      <c r="F3" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="50"/>
+      <c r="H3" s="54"/>
+      <c r="J3" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="54"/>
+      <c r="O3" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="S3" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="50"/>
+      <c r="U3" s="50"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="54"/>
+    </row>
+    <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="16"/>
+      <c r="K4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" s="61"/>
+      <c r="P4" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" s="27"/>
+      <c r="T4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U4" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" s="65" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="67.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="18">
+        <v>969599.1</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="18">
+        <v>4.9300000000000001E-9</v>
+      </c>
+      <c r="J5" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="22"/>
+      <c r="M5" s="23">
+        <f>D5/(4*H5*H6*H9)</f>
+        <v>34560.352804608599</v>
+      </c>
+      <c r="O5" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="18">
+        <v>0.28139505999999997</v>
+      </c>
+      <c r="S5" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="T5" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="U5" s="69"/>
+      <c r="V5" s="70">
+        <f>(D5 - 2*Q5)/(4*H5*H6*H9)</f>
+        <v>34560.332744539337</v>
+      </c>
+      <c r="W5" s="71">
+        <f>(D5+2*Q5)/(4*H5*H6*H9)</f>
+        <v>34560.372864677862</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="29.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="18">
+        <v>100</v>
+      </c>
+      <c r="J6" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="25"/>
+      <c r="M6" s="26">
+        <f>D6*M5</f>
+        <v>345.60352804608601</v>
+      </c>
+      <c r="O6" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" s="24">
+        <v>2.0850266999999998</v>
+      </c>
+      <c r="S6" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="T6" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="U6" s="74"/>
+      <c r="V6" s="75">
+        <f>(D6-2*Q6)*M5</f>
+        <v>-143772.91319001155</v>
+      </c>
+      <c r="W6" s="76">
+        <f>(D6+2*Q6)*M5</f>
+        <v>144464.1202461037</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="58"/>
+      <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="18"/>
+      <c r="F7" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="24">
+        <v>603301446</v>
+      </c>
+      <c r="J7" s="58"/>
+      <c r="K7" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="32"/>
+      <c r="M7" s="33">
+        <f>D7*M5</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="58"/>
+      <c r="P7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="18"/>
+      <c r="S7" s="77"/>
+      <c r="T7" s="78" t="s">
+        <v>35</v>
+      </c>
+      <c r="U7" s="32"/>
+      <c r="V7" s="79">
+        <f>(D7-2*Q7)*M5</f>
+        <v>0</v>
+      </c>
+      <c r="W7" s="33">
+        <f>(D7+2*Q7)*M5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="27.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="24">
+        <f>(15859769/599899923)*(1736464/(1839839+106915))</f>
+        <v>2.3581572371007518E-2</v>
+      </c>
+      <c r="J8" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8" s="26">
+        <f>2*D8*M5*H6</f>
+        <v>69120.705609217199</v>
+      </c>
+      <c r="O8" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="80" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q8" s="24">
+        <v>2.4788679400000002</v>
+      </c>
+      <c r="S8" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="T8" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="U8" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="V8" s="81">
+        <f>2*(D8-2*Q8)*M5*H6</f>
+        <v>-34199099.519364126</v>
+      </c>
+      <c r="W8" s="26">
+        <f>2*(D8+2*Q8)*M5*H6</f>
+        <v>34337340.930582553</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="57"/>
+      <c r="B9" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="36"/>
+      <c r="F9" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="30">
+        <f>H7*H8</f>
+        <v>14226796.710382484</v>
+      </c>
+      <c r="J9" s="57"/>
+      <c r="K9" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="38">
+        <f>2*D9*M5*H6</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="57"/>
+      <c r="P9" s="82" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q9" s="36"/>
+      <c r="S9" s="57"/>
+      <c r="T9" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="U9" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="V9" s="83">
+        <f>2*(D9-2*Q9)*M5*H6</f>
+        <v>0</v>
+      </c>
+      <c r="W9" s="38">
+        <f>2*(D9+2*Q9)*M5*H6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J10" s="55"/>
+      <c r="M10" s="41"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="J11" s="55"/>
+      <c r="M11" s="41"/>
+    </row>
+    <row r="12" spans="1:23" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="M14" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="S3:W3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
file re-org and final analyses
</commit_message>
<xml_diff>
--- a/05.analyses/demography/dadi/1D/cord/models/dadi_cord1D_results_summary.xlsx
+++ b/05.analyses/demography/dadi/1D/cord/models/dadi_cord1D_results_summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/kasey_pham_ufl_edu/Documents/Grad School Documents/Projects/eucalyptus-hybrid-resequencing/05.analyses/demography/dadi/1D/cord/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="380" documentId="8_{21408352-E5DB-40D9-AE77-F269512CD883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2471D2B4-1975-4840-8376-08477C84E082}"/>
+  <xr:revisionPtr revIDLastSave="393" documentId="8_{21408352-E5DB-40D9-AE77-F269512CD883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51583AD1-210D-4649-9C0A-7BEDF83E8DB9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{2A3D79EE-876F-4CC7-84D9-EA1A1596E616}"/>
   </bookViews>
@@ -962,54 +962,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1027,16 +979,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
@@ -1048,6 +994,60 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1063,10 +1063,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1388,8 +1384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1123D7EB-ECD6-4C25-BAEF-EFE90AE1E5C4}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1412,20 +1408,20 @@
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="45" t="s">
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="47"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="73"/>
       <c r="L1" s="9" t="s">
         <v>7</v>
       </c>
@@ -1449,7 +1445,7 @@
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="87">
+      <c r="B2" s="69">
         <v>-7399.12</v>
       </c>
       <c r="C2">
@@ -1464,7 +1460,7 @@
       <c r="F2" s="2">
         <v>-7399.13</v>
       </c>
-      <c r="G2" s="88">
+      <c r="G2" s="70">
         <v>14802.24</v>
       </c>
       <c r="H2">
@@ -1500,7 +1496,7 @@
       <c r="B3" s="43">
         <v>-7092.79</v>
       </c>
-      <c r="C3" s="85">
+      <c r="C3" s="67">
         <v>-7092.77</v>
       </c>
       <c r="D3">
@@ -1515,7 +1511,7 @@
       <c r="G3">
         <v>14189.58</v>
       </c>
-      <c r="H3" s="85">
+      <c r="H3" s="67">
         <v>14189.54</v>
       </c>
       <c r="I3">
@@ -1548,7 +1544,7 @@
       <c r="B4" s="43">
         <v>-7388.91</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="68">
         <v>-7358.44</v>
       </c>
       <c r="D4">
@@ -1563,7 +1559,7 @@
       <c r="G4">
         <v>14783.82</v>
       </c>
-      <c r="H4" s="86">
+      <c r="H4" s="68">
         <v>14722.88</v>
       </c>
       <c r="I4">
@@ -1599,7 +1595,7 @@
       <c r="B5" s="44">
         <v>-6552</v>
       </c>
-      <c r="C5" s="84">
+      <c r="C5" s="66">
         <v>-5272.02</v>
       </c>
       <c r="D5" s="3">
@@ -1614,7 +1610,7 @@
       <c r="G5" s="3">
         <v>13112</v>
       </c>
-      <c r="H5" s="84">
+      <c r="H5" s="66">
         <v>10552.04</v>
       </c>
       <c r="I5" s="3">
@@ -1689,42 +1685,42 @@
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="52"/>
-      <c r="F3" s="53" t="s">
+      <c r="B3" s="76"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="86"/>
+      <c r="F3" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="50"/>
-      <c r="H3" s="54"/>
-      <c r="J3" s="53" t="s">
+      <c r="G3" s="76"/>
+      <c r="H3" s="77"/>
+      <c r="J3" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="54"/>
-      <c r="O3" s="60" t="s">
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="77"/>
+      <c r="O3" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
-      <c r="S3" s="53" t="s">
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="S3" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="54"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="77"/>
     </row>
     <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10"/>
@@ -1756,24 +1752,24 @@
       <c r="M4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="61"/>
-      <c r="P4" s="62" t="s">
+      <c r="O4" s="45"/>
+      <c r="P4" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="63" t="s">
+      <c r="Q4" s="47" t="s">
         <v>19</v>
       </c>
       <c r="S4" s="27"/>
       <c r="T4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U4" s="64" t="s">
+      <c r="U4" s="48" t="s">
         <v>18</v>
       </c>
       <c r="V4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="W4" s="65" t="s">
+      <c r="W4" s="49" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1808,31 +1804,31 @@
         <f>D5/(4*H5*H6*H9)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="66" t="s">
+      <c r="O5" s="50" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="Q5" s="18"/>
-      <c r="S5" s="67" t="s">
+      <c r="S5" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="T5" s="68" t="s">
+      <c r="T5" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="U5" s="69"/>
-      <c r="V5" s="70">
+      <c r="U5" s="53"/>
+      <c r="V5" s="54">
         <f>(D5 - 2*Q5)/(4*H5*H6*H9)</f>
         <v>0</v>
       </c>
-      <c r="W5" s="71">
+      <c r="W5" s="55">
         <f>(D5+2*Q5)/(4*H5*H6*H9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="29.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="78" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">
@@ -1849,7 +1845,7 @@
       <c r="H6" s="18">
         <v>100</v>
       </c>
-      <c r="J6" s="56" t="s">
+      <c r="J6" s="78" t="s">
         <v>24</v>
       </c>
       <c r="K6" s="40" t="s">
@@ -1860,31 +1856,31 @@
         <f>D6*M5</f>
         <v>0</v>
       </c>
-      <c r="O6" s="56" t="s">
+      <c r="O6" s="78" t="s">
         <v>24</v>
       </c>
       <c r="P6" s="2" t="s">
         <v>34</v>
       </c>
       <c r="Q6" s="24"/>
-      <c r="S6" s="72" t="s">
+      <c r="S6" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="T6" s="73" t="s">
+      <c r="T6" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="U6" s="74"/>
-      <c r="V6" s="75">
+      <c r="U6" s="57"/>
+      <c r="V6" s="58">
         <f>(D6-2*Q6)*M5</f>
         <v>0</v>
       </c>
-      <c r="W6" s="76">
+      <c r="W6" s="59">
         <f>(D6+2*Q6)*M5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="58"/>
+      <c r="A7" s="79"/>
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
@@ -1899,7 +1895,7 @@
       <c r="H7" s="24">
         <v>603301446</v>
       </c>
-      <c r="J7" s="58"/>
+      <c r="J7" s="79"/>
       <c r="K7" s="31" t="s">
         <v>35</v>
       </c>
@@ -1908,17 +1904,17 @@
         <f>D7*M5</f>
         <v>0</v>
       </c>
-      <c r="O7" s="58"/>
+      <c r="O7" s="79"/>
       <c r="P7" s="4" t="s">
         <v>35</v>
       </c>
       <c r="Q7" s="18"/>
-      <c r="S7" s="77"/>
-      <c r="T7" s="78" t="s">
+      <c r="S7" s="81"/>
+      <c r="T7" s="60" t="s">
         <v>35</v>
       </c>
       <c r="U7" s="32"/>
-      <c r="V7" s="79">
+      <c r="V7" s="61">
         <f>(D7-2*Q7)*M5</f>
         <v>0</v>
       </c>
@@ -1928,7 +1924,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="27.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="78" t="s">
         <v>32</v>
       </c>
       <c r="B8" t="s">
@@ -1944,7 +1940,7 @@
         <f>(15859769/599899923)*(1736464/(1839839+106915))</f>
         <v>2.3581572371007518E-2</v>
       </c>
-      <c r="J8" s="56" t="s">
+      <c r="J8" s="78" t="s">
         <v>32</v>
       </c>
       <c r="K8" s="40" t="s">
@@ -1957,14 +1953,14 @@
         <f>2*D8*M5*H6</f>
         <v>0</v>
       </c>
-      <c r="O8" s="56" t="s">
+      <c r="O8" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="P8" s="80" t="s">
+      <c r="P8" s="62" t="s">
         <v>36</v>
       </c>
       <c r="Q8" s="24"/>
-      <c r="S8" s="56" t="s">
+      <c r="S8" s="78" t="s">
         <v>32</v>
       </c>
       <c r="T8" s="40" t="s">
@@ -1973,7 +1969,7 @@
       <c r="U8" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="V8" s="81">
+      <c r="V8" s="63">
         <f>2*(D8-2*Q8)*M5*H6</f>
         <v>0</v>
       </c>
@@ -1983,7 +1979,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="57"/>
+      <c r="A9" s="82"/>
       <c r="B9" s="34" t="s">
         <v>37</v>
       </c>
@@ -1999,7 +1995,7 @@
         <f>H7*H8</f>
         <v>14226796.710382484</v>
       </c>
-      <c r="J9" s="57"/>
+      <c r="J9" s="82"/>
       <c r="K9" s="37" t="s">
         <v>37</v>
       </c>
@@ -2010,19 +2006,19 @@
         <f>2*D9*M5*H6</f>
         <v>0</v>
       </c>
-      <c r="O9" s="57"/>
-      <c r="P9" s="82" t="s">
+      <c r="O9" s="82"/>
+      <c r="P9" s="64" t="s">
         <v>37</v>
       </c>
       <c r="Q9" s="36"/>
-      <c r="S9" s="57"/>
+      <c r="S9" s="82"/>
       <c r="T9" s="37" t="s">
         <v>48</v>
       </c>
       <c r="U9" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="V9" s="83">
+      <c r="V9" s="65">
         <f>2*(D9-2*Q9)*M5*H6</f>
         <v>0</v>
       </c>
@@ -2032,11 +2028,11 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="J10" s="55"/>
+      <c r="J10" s="87"/>
       <c r="M10" s="41"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="J11" s="55"/>
+      <c r="J11" s="87"/>
       <c r="M11" s="41"/>
     </row>
     <row r="12" spans="1:23" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2047,12 +2043,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="S3:W3"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="S8:S9"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="F3:H3"/>
@@ -2062,6 +2052,12 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="J6:J7"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="S3:W3"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="S8:S9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2072,7 +2068,7 @@
   <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2101,44 +2097,44 @@
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="52"/>
-      <c r="F3" s="53" t="s">
+      <c r="B3" s="76"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="86"/>
+      <c r="F3" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="50"/>
-      <c r="H3" s="54"/>
-      <c r="J3" s="53" t="s">
+      <c r="G3" s="76"/>
+      <c r="H3" s="77"/>
+      <c r="J3" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="54"/>
-      <c r="O3" s="60" t="s">
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="77"/>
+      <c r="O3" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
-      <c r="S3" s="53" t="s">
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="S3" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="54"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="77"/>
     </row>
     <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10"/>
@@ -2170,24 +2166,24 @@
       <c r="M4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="61"/>
-      <c r="P4" s="62" t="s">
+      <c r="O4" s="45"/>
+      <c r="P4" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="63" t="s">
+      <c r="Q4" s="47" t="s">
         <v>19</v>
       </c>
       <c r="S4" s="27"/>
       <c r="T4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U4" s="64" t="s">
+      <c r="U4" s="48" t="s">
         <v>18</v>
       </c>
       <c r="V4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="W4" s="65" t="s">
+      <c r="W4" s="49" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2225,31 +2221,31 @@
         <f>D5/(4*H5*H6*H9)</f>
         <v>32587.138750562626</v>
       </c>
-      <c r="O5" s="66" t="s">
+      <c r="O5" s="50" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="Q5" s="18"/>
-      <c r="S5" s="67" t="s">
+      <c r="S5" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="T5" s="68" t="s">
+      <c r="T5" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="U5" s="69"/>
-      <c r="V5" s="70">
+      <c r="U5" s="53"/>
+      <c r="V5" s="54">
         <f>(D5 - 2*Q5)/(4*H5*H6*H9)</f>
         <v>32587.138750562626</v>
       </c>
-      <c r="W5" s="71">
+      <c r="W5" s="55">
         <f>(D5+2*Q5)/(4*H5*H6*H9)</f>
         <v>32587.138750562626</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="29.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="78" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">
@@ -2268,7 +2264,7 @@
       <c r="H6" s="18">
         <v>100</v>
       </c>
-      <c r="J6" s="56" t="s">
+      <c r="J6" s="78" t="s">
         <v>24</v>
       </c>
       <c r="K6" s="40" t="s">
@@ -2279,31 +2275,31 @@
         <f>D6*M5</f>
         <v>865726.22161682206</v>
       </c>
-      <c r="O6" s="56" t="s">
+      <c r="O6" s="78" t="s">
         <v>24</v>
       </c>
       <c r="P6" s="2" t="s">
         <v>34</v>
       </c>
       <c r="Q6" s="24"/>
-      <c r="S6" s="72" t="s">
+      <c r="S6" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="T6" s="73" t="s">
+      <c r="T6" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="U6" s="74"/>
-      <c r="V6" s="75">
+      <c r="U6" s="57"/>
+      <c r="V6" s="58">
         <f>(D6-2*Q6)*M5</f>
         <v>865726.22161682206</v>
       </c>
-      <c r="W6" s="76">
+      <c r="W6" s="59">
         <f>(D6+2*Q6)*M5</f>
         <v>865726.22161682206</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="58"/>
+      <c r="A7" s="79"/>
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
@@ -2320,7 +2316,7 @@
       <c r="H7" s="24">
         <v>603301446</v>
       </c>
-      <c r="J7" s="58"/>
+      <c r="J7" s="79"/>
       <c r="K7" s="31" t="s">
         <v>35</v>
       </c>
@@ -2329,17 +2325,17 @@
         <f>D7*M5</f>
         <v>329.1301013806825</v>
       </c>
-      <c r="O7" s="58"/>
+      <c r="O7" s="79"/>
       <c r="P7" s="4" t="s">
         <v>35</v>
       </c>
       <c r="Q7" s="18"/>
-      <c r="S7" s="77"/>
-      <c r="T7" s="78" t="s">
+      <c r="S7" s="81"/>
+      <c r="T7" s="60" t="s">
         <v>35</v>
       </c>
       <c r="U7" s="32"/>
-      <c r="V7" s="79">
+      <c r="V7" s="61">
         <f>(D7-2*Q7)*M5</f>
         <v>329.1301013806825</v>
       </c>
@@ -2349,7 +2345,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="27.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="78" t="s">
         <v>32</v>
       </c>
       <c r="B8" t="s">
@@ -2367,7 +2363,7 @@
         <f>(15859769/599899923)*(1736464/(1839839+106915))</f>
         <v>2.3581572371007518E-2</v>
       </c>
-      <c r="J8" s="56" t="s">
+      <c r="J8" s="78" t="s">
         <v>32</v>
       </c>
       <c r="K8" s="40" t="s">
@@ -2380,14 +2376,14 @@
         <f>2*D8*M5*H6</f>
         <v>156192111.2597717</v>
       </c>
-      <c r="O8" s="56" t="s">
+      <c r="O8" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="P8" s="80" t="s">
+      <c r="P8" s="62" t="s">
         <v>36</v>
       </c>
       <c r="Q8" s="24"/>
-      <c r="S8" s="56" t="s">
+      <c r="S8" s="78" t="s">
         <v>32</v>
       </c>
       <c r="T8" s="40" t="s">
@@ -2396,7 +2392,7 @@
       <c r="U8" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="V8" s="81">
+      <c r="V8" s="63">
         <f>2*(D8-2*Q8)*M5*H6</f>
         <v>156192111.2597717</v>
       </c>
@@ -2406,7 +2402,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="57"/>
+      <c r="A9" s="82"/>
       <c r="B9" s="34" t="s">
         <v>37</v>
       </c>
@@ -2424,7 +2420,7 @@
         <f>H7*H8</f>
         <v>14226796.710382484</v>
       </c>
-      <c r="J9" s="57"/>
+      <c r="J9" s="82"/>
       <c r="K9" s="37" t="s">
         <v>37</v>
       </c>
@@ -2435,19 +2431,19 @@
         <f>2*D9*M5*H6</f>
         <v>91895.731276586608</v>
       </c>
-      <c r="O9" s="57"/>
-      <c r="P9" s="82" t="s">
+      <c r="O9" s="82"/>
+      <c r="P9" s="64" t="s">
         <v>37</v>
       </c>
       <c r="Q9" s="36"/>
-      <c r="S9" s="57"/>
+      <c r="S9" s="82"/>
       <c r="T9" s="37" t="s">
         <v>48</v>
       </c>
       <c r="U9" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="V9" s="83">
+      <c r="V9" s="65">
         <f>2*(D9-2*Q9)*M5*H6</f>
         <v>91895.731276586608</v>
       </c>
@@ -2457,11 +2453,11 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="J10" s="55"/>
+      <c r="J10" s="87"/>
       <c r="M10" s="41"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="J11" s="55"/>
+      <c r="J11" s="87"/>
       <c r="M11" s="41"/>
     </row>
     <row r="12" spans="1:23" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2472,12 +2468,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="S3:W3"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="S8:S9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="J10:J11"/>
@@ -2487,6 +2477,12 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="J6:J7"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="S3:W3"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="S8:S9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2496,8 +2492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED4A405-5A85-4992-8768-5EA27FBA628E}">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2527,44 +2523,44 @@
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="88" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="52"/>
-      <c r="F3" s="53" t="s">
+      <c r="B3" s="76"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="86"/>
+      <c r="F3" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="50"/>
-      <c r="H3" s="54"/>
-      <c r="J3" s="53" t="s">
+      <c r="G3" s="76"/>
+      <c r="H3" s="77"/>
+      <c r="J3" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="54"/>
-      <c r="O3" s="60" t="s">
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="77"/>
+      <c r="O3" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
-      <c r="S3" s="53" t="s">
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="S3" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="54"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="77"/>
     </row>
     <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10"/>
@@ -2596,24 +2592,24 @@
       <c r="M4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="61"/>
-      <c r="P4" s="62" t="s">
+      <c r="O4" s="45"/>
+      <c r="P4" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="63" t="s">
+      <c r="Q4" s="47" t="s">
         <v>19</v>
       </c>
       <c r="S4" s="27"/>
       <c r="T4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U4" s="64" t="s">
+      <c r="U4" s="48" t="s">
         <v>18</v>
       </c>
       <c r="V4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="W4" s="65" t="s">
+      <c r="W4" s="49" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2637,9 +2633,9 @@
         <v>23</v>
       </c>
       <c r="H5" s="18">
-        <v>4.9300000000000001E-9</v>
-      </c>
-      <c r="J5" s="42" t="s">
+        <v>4.9299999999999995E-10</v>
+      </c>
+      <c r="J5" s="50" t="s">
         <v>20</v>
       </c>
       <c r="K5" s="21" t="s">
@@ -2648,9 +2644,9 @@
       <c r="L5" s="22"/>
       <c r="M5" s="23">
         <f>D5/(4*H5*H6*H9)</f>
-        <v>34560.352804608599</v>
-      </c>
-      <c r="O5" s="66" t="s">
+        <v>345603.52804608602</v>
+      </c>
+      <c r="O5" s="50" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="4" t="s">
@@ -2659,24 +2655,24 @@
       <c r="Q5" s="18">
         <v>0.28139505999999997</v>
       </c>
-      <c r="S5" s="67" t="s">
+      <c r="S5" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="T5" s="68" t="s">
+      <c r="T5" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="U5" s="69"/>
-      <c r="V5" s="70">
+      <c r="U5" s="53"/>
+      <c r="V5" s="54">
         <f>(D5 - 2*Q5)/(4*H5*H6*H9)</f>
-        <v>34560.332744539337</v>
-      </c>
-      <c r="W5" s="71">
+        <v>345603.32744539337</v>
+      </c>
+      <c r="W5" s="55">
         <f>(D5+2*Q5)/(4*H5*H6*H9)</f>
-        <v>34560.372864677862</v>
+        <v>345603.72864677862</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="29.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="78" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">
@@ -2695,7 +2691,7 @@
       <c r="H6" s="18">
         <v>100</v>
       </c>
-      <c r="J6" s="56" t="s">
+      <c r="J6" s="78" t="s">
         <v>24</v>
       </c>
       <c r="K6" s="40" t="s">
@@ -2704,9 +2700,9 @@
       <c r="L6" s="25"/>
       <c r="M6" s="26">
         <f>D6*M5</f>
-        <v>345.60352804608601</v>
-      </c>
-      <c r="O6" s="56" t="s">
+        <v>3456.0352804608601</v>
+      </c>
+      <c r="O6" s="78" t="s">
         <v>24</v>
       </c>
       <c r="P6" s="2" t="s">
@@ -2715,24 +2711,24 @@
       <c r="Q6" s="24">
         <v>2.0850266999999998</v>
       </c>
-      <c r="S6" s="72" t="s">
+      <c r="S6" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="T6" s="73" t="s">
+      <c r="T6" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="U6" s="74"/>
-      <c r="V6" s="75">
+      <c r="U6" s="57"/>
+      <c r="V6" s="58">
         <f>(D6-2*Q6)*M5</f>
-        <v>-143772.91319001155</v>
-      </c>
-      <c r="W6" s="76">
+        <v>-1437729.1319001154</v>
+      </c>
+      <c r="W6" s="59">
         <f>(D6+2*Q6)*M5</f>
-        <v>144464.1202461037</v>
+        <v>1444641.2024610371</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="58"/>
+      <c r="A7" s="79"/>
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
@@ -2747,7 +2743,7 @@
       <c r="H7" s="24">
         <v>603301446</v>
       </c>
-      <c r="J7" s="58"/>
+      <c r="J7" s="79"/>
       <c r="K7" s="31" t="s">
         <v>35</v>
       </c>
@@ -2756,17 +2752,17 @@
         <f>D7*M5</f>
         <v>0</v>
       </c>
-      <c r="O7" s="58"/>
+      <c r="O7" s="79"/>
       <c r="P7" s="4" t="s">
         <v>35</v>
       </c>
       <c r="Q7" s="18"/>
-      <c r="S7" s="77"/>
-      <c r="T7" s="78" t="s">
+      <c r="S7" s="81"/>
+      <c r="T7" s="60" t="s">
         <v>35</v>
       </c>
       <c r="U7" s="32"/>
-      <c r="V7" s="79">
+      <c r="V7" s="61">
         <f>(D7-2*Q7)*M5</f>
         <v>0</v>
       </c>
@@ -2776,7 +2772,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="27.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="78" t="s">
         <v>32</v>
       </c>
       <c r="B8" t="s">
@@ -2794,7 +2790,7 @@
         <f>(15859769/599899923)*(1736464/(1839839+106915))</f>
         <v>2.3581572371007518E-2</v>
       </c>
-      <c r="J8" s="56" t="s">
+      <c r="J8" s="78" t="s">
         <v>32</v>
       </c>
       <c r="K8" s="40" t="s">
@@ -2805,18 +2801,18 @@
       </c>
       <c r="M8" s="26">
         <f>2*D8*M5*H6</f>
-        <v>69120.705609217199</v>
-      </c>
-      <c r="O8" s="56" t="s">
+        <v>691207.05609217205</v>
+      </c>
+      <c r="O8" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="P8" s="80" t="s">
+      <c r="P8" s="62" t="s">
         <v>36</v>
       </c>
       <c r="Q8" s="24">
         <v>2.4788679400000002</v>
       </c>
-      <c r="S8" s="56" t="s">
+      <c r="S8" s="78" t="s">
         <v>32</v>
       </c>
       <c r="T8" s="40" t="s">
@@ -2825,17 +2821,17 @@
       <c r="U8" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="V8" s="81">
+      <c r="V8" s="63">
         <f>2*(D8-2*Q8)*M5*H6</f>
-        <v>-34199099.519364126</v>
+        <v>-341990995.19364125</v>
       </c>
       <c r="W8" s="26">
         <f>2*(D8+2*Q8)*M5*H6</f>
-        <v>34337340.930582553</v>
+        <v>343373409.30582559</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="57"/>
+      <c r="A9" s="82"/>
       <c r="B9" s="34" t="s">
         <v>37</v>
       </c>
@@ -2851,7 +2847,7 @@
         <f>H7*H8</f>
         <v>14226796.710382484</v>
       </c>
-      <c r="J9" s="57"/>
+      <c r="J9" s="82"/>
       <c r="K9" s="37" t="s">
         <v>37</v>
       </c>
@@ -2862,19 +2858,19 @@
         <f>2*D9*M5*H6</f>
         <v>0</v>
       </c>
-      <c r="O9" s="57"/>
-      <c r="P9" s="82" t="s">
+      <c r="O9" s="82"/>
+      <c r="P9" s="64" t="s">
         <v>37</v>
       </c>
       <c r="Q9" s="36"/>
-      <c r="S9" s="57"/>
+      <c r="S9" s="82"/>
       <c r="T9" s="37" t="s">
         <v>48</v>
       </c>
       <c r="U9" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="V9" s="83">
+      <c r="V9" s="65">
         <f>2*(D9-2*Q9)*M5*H6</f>
         <v>0</v>
       </c>
@@ -2884,11 +2880,11 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="J10" s="55"/>
+      <c r="J10" s="87"/>
       <c r="M10" s="41"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="J11" s="55"/>
+      <c r="J11" s="87"/>
       <c r="M11" s="41"/>
     </row>
     <row r="12" spans="1:23" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2899,6 +2895,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="S3:W3"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="O3:Q3"/>
     <mergeCell ref="J10:J11"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="J6:J7"/>
@@ -2908,12 +2910,6 @@
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="O8:O9"/>
     <mergeCell ref="S8:S9"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="S3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>